<commit_message>
Clean up entire repository
- Link ReadMe to published Manuscript
- Change figures numbering to the one used in the MS
- Test all code
- Recalculate all figures
- Remove numbers from Fig 1
</commit_message>
<xml_diff>
--- a/results/TABLE_2-summary-review.xlsx
+++ b/results/TABLE_2-summary-review.xlsx
@@ -1,109 +1,87 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10615"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tobias/Documents/Dropbox/Schreibtisch_Ro/1568_Publi-NDep-Tagfalter/10-GitHub-NDep_butterflies/results/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{287EFC57-74C8-F646-A291-49E48B3C763F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <workbookPr date1904="false"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="21780" windowHeight="14500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>Subcategory</t>
-  </si>
-  <si>
-    <t>Number of variables</t>
-  </si>
-  <si>
-    <t>Studies</t>
-  </si>
-  <si>
-    <t>Importance</t>
-  </si>
-  <si>
-    <t>Direction</t>
-  </si>
-  <si>
-    <t>Environment</t>
-  </si>
-  <si>
-    <t>Climate-Gradient</t>
-  </si>
-  <si>
-    <t>Climate-Variability</t>
-  </si>
-  <si>
-    <t>Topography</t>
-  </si>
-  <si>
-    <t>Habitat</t>
-  </si>
-  <si>
-    <t>Habitat configuration</t>
-  </si>
-  <si>
-    <t>Habitat diversity</t>
-  </si>
-  <si>
-    <t>Habitat-availability</t>
-  </si>
-  <si>
-    <t>Land-use intensity</t>
-  </si>
-  <si>
-    <t>Vegetation</t>
-  </si>
-  <si>
-    <t>Microclimate</t>
-  </si>
-  <si>
-    <t>Resource diversity</t>
-  </si>
-  <si>
-    <t>Others</t>
-  </si>
-  <si>
-    <t>–</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+  <si>
+    <t xml:space="preserve">Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subcategory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of predictor variables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of studies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Importance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Direction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Environment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Climate-Gradient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Climate-Variability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Topography</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Habitat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Habitat configuration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Habitat diversity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Habitat-availability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Land-use intensity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vegetation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Microclimate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resource diversity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Others</t>
+  </si>
+  <si>
+    <t xml:space="preserve">–</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -118,7 +96,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -126,49 +104,17 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -450,245 +396,235 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F11"/>
-    </sheetView>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.6640625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="2">
+      <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" t="n">
         <v>10</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" t="n">
         <v>18</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" t="n">
         <v>0.63</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" t="n">
         <v>0.26</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+    <row r="3">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" t="n">
         <v>4</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" t="n">
         <v>8</v>
       </c>
-      <c r="E3" s="2">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="F3" s="2">
+      <c r="E3" t="n">
+        <v>0.56</v>
+      </c>
+      <c r="F3" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+    <row r="4">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" t="n">
         <v>3</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" t="n">
         <v>13</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" t="n">
         <v>0.45</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" t="n">
         <v>0.19</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+    <row r="5">
+      <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" t="n">
         <v>6</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" t="n">
         <v>7</v>
       </c>
-      <c r="E5" s="2">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="F5" s="2">
+      <c r="E5" t="n">
+        <v>0.58</v>
+      </c>
+      <c r="F5" t="n">
         <v>-0.1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+    <row r="6">
+      <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" t="n">
         <v>4</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" t="n">
         <v>11</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" t="n">
         <v>0.64</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" t="n">
         <v>0.27</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+    <row r="7">
+      <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" t="n">
         <v>11</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" t="n">
         <v>20</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" t="n">
         <v>0.64</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" t="n">
         <v>0.15</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+    <row r="8">
+      <c r="A8" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" t="n">
         <v>25</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" t="n">
         <v>19</v>
       </c>
-      <c r="E8" s="2">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="F8" s="2">
+      <c r="E8" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="F8" t="n">
         <v>-0.42</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+    <row r="9">
+      <c r="A9" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" t="n">
         <v>3</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" t="n">
         <v>7</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" t="n">
         <v>0.64</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" t="n">
         <v>0.11</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+    <row r="10">
+      <c r="A10" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" t="n">
         <v>8</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" t="n">
         <v>13</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" t="n">
         <v>0.59</v>
       </c>
-      <c r="F10" s="2">
-        <v>0.56999999999999995</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
+      <c r="F10" t="n">
+        <v>0.57</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" t="n">
         <v>4</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" t="n">
         <v>6</v>
       </c>
-      <c r="E11" s="3">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="F11" s="3">
+      <c r="E11" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="F11" t="n">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>